<commit_message>
Set author to "SAP Cloud ALM"
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
+++ b/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I500371/SAPDevelop/git/others/github/SAP-samples/cloud-alm-api-examples/spreadsheet-examples/spreadsheet-testcases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E3ED1A-1994-2049-BADC-0285D2CEB809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB6FBC8-1474-A94D-AF4C-BBD9B0BA0704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21280" xr2:uid="{319E5F16-275C-DC4F-8D16-517661E09C6E}"/>
   </bookViews>
@@ -326,11 +326,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -829,7 +829,7 @@
       <c r="H5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>47</v>
       </c>
       <c r="J5" s="4" t="s">
@@ -1008,16 +1008,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated sap help link and title
mail address example removed
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
+++ b/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I500371/SAPDevelop/git/others/github/SAP-samples/cloud-alm-api-examples/spreadsheet-examples/spreadsheet-testcases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB6FBC8-1474-A94D-AF4C-BBD9B0BA0704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C081268D-3D53-0140-8A22-DC7EB3FF23FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21280" xr2:uid="{319E5F16-275C-DC4F-8D16-517661E09C6E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Medium</t>
-  </si>
-  <si>
-    <t>user@example.com</t>
   </si>
   <si>
     <t>https://sap.com</t>
@@ -180,9 +177,6 @@
     <t>Application 2</t>
   </si>
   <si>
-    <t>For detailed information on the creation of documents via spreadsheet, see SAP Help Portal.</t>
-  </si>
-  <si>
     <t>https://help.sap.com</t>
   </si>
   <si>
@@ -192,6 +186,9 @@
   <si>
     <t>TagA
 TagB</t>
+  </si>
+  <si>
+    <t>For detailed information on the creation of test cases via spreadsheet, see SAP Help Portal.</t>
   </si>
 </sst>
 </file>
@@ -671,7 +668,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -702,10 +699,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>9</v>
@@ -731,7 +728,7 @@
     </row>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>10</v>
@@ -740,136 +737,132 @@
         <v>11</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>13</v>
-      </c>
       <c r="J2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="7"/>
       <c r="E3" s="10"/>
       <c r="G3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="E5" s="10"/>
       <c r="G5" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="J5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="E6" s="10"/>
       <c r="G6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="E7" s="10"/>
       <c r="G7" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="11" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
@@ -900,11 +893,9 @@
     <row r="33" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{A749A97B-556C-144D-805F-C69AAE86C2DA}"/>
-    <hyperlink ref="I2" r:id="rId2" xr:uid="{D34F3B38-561F-E94E-AEEA-BD5FE771015A}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{BFA51C5B-3153-2A49-B2B0-BB4B94FCD2E0}"/>
-    <hyperlink ref="I4" r:id="rId4" xr:uid="{8498B9AE-B875-B047-9460-2132C8DE10CD}"/>
-    <hyperlink ref="I5" r:id="rId5" xr:uid="{2346ADE1-55B3-4349-B3BB-7C3B3BED0E9D}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{D34F3B38-561F-E94E-AEEA-BD5FE771015A}"/>
+    <hyperlink ref="I4" r:id="rId2" xr:uid="{8498B9AE-B875-B047-9460-2132C8DE10CD}"/>
+    <hyperlink ref="I5" r:id="rId3" xr:uid="{2346ADE1-55B3-4349-B3BB-7C3B3BED0E9D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -925,7 +916,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -933,12 +924,12 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -962,17 +953,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -980,12 +971,12 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1009,7 +1000,7 @@
   <sheetData>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
@@ -1025,7 +1016,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1" display="SAP Help Portal." xr:uid="{729BC32D-1540-4C46-BEE9-0662F4D3C8D8}"/>
-    <hyperlink ref="A4:H4" r:id="rId2" display="For detailed information on the creation of documents via spreadsheet, see SAP Help Portal." xr:uid="{3943A47B-CC35-CB48-BB16-32E1C835DFFA}"/>
+    <hyperlink ref="A4:H4" r:id="rId2" display="For detailed information on the creation of test cases via spreadsheet, see SAP Help Portal." xr:uid="{3943A47B-CC35-CB48-BB16-32E1C835DFFA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove private data setting included
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
+++ b/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
@@ -2,13 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I500371/SAPDevelop/git/others/github/SAP-samples/cloud-alm-api-examples/spreadsheet-examples/spreadsheet-testcases/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C081268D-3D53-0140-8A22-DC7EB3FF23FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3B125-14DA-6040-9894-FA5FD3C25941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21280" xr2:uid="{319E5F16-275C-DC4F-8D16-517661E09C6E}"/>
   </bookViews>

</xml_diff>

<commit_message>
example for owner added
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
+++ b/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B3B125-14DA-6040-9894-FA5FD3C25941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1633BBA2-3391-7F4B-A628-6C85A32FA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21280" xr2:uid="{319E5F16-275C-DC4F-8D16-517661E09C6E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>For detailed information on the creation of test cases via spreadsheet, see SAP Help Portal.</t>
+  </si>
+  <si>
+    <t>owner@sap.com</t>
   </si>
 </sst>
 </file>
@@ -663,7 +666,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -734,7 +737,9 @@
       <c r="D2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="F2" s="9" t="s">
         <v>46</v>
       </c>
@@ -891,6 +896,7 @@
     <hyperlink ref="I2" r:id="rId1" xr:uid="{D34F3B38-561F-E94E-AEEA-BD5FE771015A}"/>
     <hyperlink ref="I4" r:id="rId2" xr:uid="{8498B9AE-B875-B047-9460-2132C8DE10CD}"/>
     <hyperlink ref="I5" r:id="rId3" xr:uid="{2346ADE1-55B3-4349-B3BB-7C3B3BED0E9D}"/>
+    <hyperlink ref="E2" r:id="rId4" xr:uid="{5D72A699-8A59-8045-AEFF-263767779B4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjusted Help Portal Link
adjusted link to Help Portal
</commit_message>
<xml_diff>
--- a/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
+++ b/spreadsheet-examples/spreadsheet-testcases/SAP Cloud ALM - Test Cases template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1633BBA2-3391-7F4B-A628-6C85A32FA38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB52DA5-DE14-6642-A2C7-DC7156A15706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21280" xr2:uid="{319E5F16-275C-DC4F-8D16-517661E09C6E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26600" activeTab="3" xr2:uid="{319E5F16-275C-DC4F-8D16-517661E09C6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F074F545-8DF7-574C-A052-283E801768E5}">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -993,8 +993,8 @@
   </sheetPr>
   <dimension ref="A4:H4"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>